<commit_message>
commit last date. Monday will run
</commit_message>
<xml_diff>
--- a/TCCB-ThuyenChuyen-TuyenDung/TCCB_QuanLy/Utils/ds-hople-tuyendung.xlsx
+++ b/TCCB-ThuyenChuyen-TuyenDung/TCCB_QuanLy/Utils/ds-hople-tuyendung.xlsx
@@ -5,19 +5,19 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="7 2 2019 12 00 00 AM" sheetId="1" r:id="rId1"/>
+    <sheet name="7 7 2019 12 00 00 AM" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="199">
   <si>
     <t>DANH SÁCH ỨNG VIÊN CÓ HỒ SƠ HỢP LỆ</t>
   </si>
   <si>
-    <t>Tính tới ngày 02/07/2019</t>
+    <t>Tính tới ngày 07/07/2019</t>
   </si>
   <si>
     <t>MÃ</t>
@@ -143,104 +143,478 @@
     <t>NGÀY RÀ XOÁT</t>
   </si>
   <si>
-    <t>TD6</t>
-  </si>
-  <si>
-    <t>Tin học</t>
-  </si>
-  <si>
-    <t>Thành Trương Hữu</t>
-  </si>
-  <si>
-    <t>10/02/1995</t>
+    <t>TD14</t>
+  </si>
+  <si>
+    <t>Giáo dục công dân</t>
+  </si>
+  <si>
+    <t>THÔNG MINH TÈO</t>
+  </si>
+  <si>
+    <t>18/10/1994</t>
   </si>
   <si>
     <t>Nam</t>
   </si>
   <si>
+    <t>Chăm</t>
+  </si>
+  <si>
+    <t>Bà La Môn</t>
+  </si>
+  <si>
+    <t>261381557</t>
+  </si>
+  <si>
+    <t>26/05/2017</t>
+  </si>
+  <si>
+    <t>Tỉnh Bình Thuận</t>
+  </si>
+  <si>
+    <t>0389014548</t>
+  </si>
+  <si>
+    <t>thongminhteo@gmail.com</t>
+  </si>
+  <si>
+    <t>Số 30/9, Thôn 3, Phường Hiệp Bình Chánh, Quận Thủ Đức, Thành Phố Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>Số 30/9, Thôn 3, Thị Trấn Ma Lâm, Huyện Hàm Thuận Bắc, Tỉnh Bình Thuận</t>
+  </si>
+  <si>
+    <t>Bình thường</t>
+  </si>
+  <si>
+    <t>Khác</t>
+  </si>
+  <si>
+    <t>Tốt nghiệp Đại học chuyên ngành sư phạm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giáo dục Chính trị
+</t>
+  </si>
+  <si>
+    <t>Chính quy</t>
+  </si>
+  <si>
+    <t>Trường Đại học Sư phạm Tp. Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>Thành Phố Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>Tín chỉ</t>
+  </si>
+  <si>
+    <t>Khá</t>
+  </si>
+  <si>
+    <t>1155587</t>
+  </si>
+  <si>
+    <t>Không</t>
+  </si>
+  <si>
+    <t>Chứng chỉ Ứng dụng CNTT cơ bàn</t>
+  </si>
+  <si>
+    <t>0934665</t>
+  </si>
+  <si>
+    <t>Bậc 2/ Trình độ B/ Trình độ A2/ Preliminary KET/ BULATS 20/ TOEFL iBT 40/ TOEIC 225</t>
+  </si>
+  <si>
+    <t>A2043214</t>
+  </si>
+  <si>
+    <t>Người dân tộc thiểu số, sĩ quan quân đội, sĩ quan công an, quân nhân chuyên nghiệp, người làm công tác cơ yếu chuyển ngành, con liệt sĩ, con thương binh, con bệnh binh, con của người hưởng chính sách như thương binh, con của thương binh loại B, con của người hoạt động cách mạng trước tổng khởi nghĩa (từ ngày 19 tháng 8 năm 1945 trở về trước), con đẻ của người hoạt động kháng chiến bị nhiễm chất độc hóa học, con Anh hùng Lực lượng vũ trang, con Anh hùng Lao động</t>
+  </si>
+  <si>
+    <t>Quận Bình Thạnh</t>
+  </si>
+  <si>
+    <t>Quận Thủ Đức</t>
+  </si>
+  <si>
+    <t>Quận Gò Vấp</t>
+  </si>
+  <si>
+    <t>HT19_1</t>
+  </si>
+  <si>
+    <t>07/07/2019</t>
+  </si>
+  <si>
+    <t>TD15</t>
+  </si>
+  <si>
+    <t>Thể dục</t>
+  </si>
+  <si>
+    <t>NGUYỄN THÂN HỮU TÍN</t>
+  </si>
+  <si>
+    <t>27/01/1997</t>
+  </si>
+  <si>
     <t>Kinh</t>
   </si>
   <si>
-    <t>Không</t>
-  </si>
-  <si>
-    <t>123456789</t>
-  </si>
-  <si>
-    <t>30/01/2010</t>
-  </si>
-  <si>
-    <t>Thành Phố Hồ Chí Minh</t>
-  </si>
-  <si>
-    <t>0988670449</t>
-  </si>
-  <si>
-    <t>truonghuuthanh95@gmail.com</t>
+    <t>Thiên chúa</t>
+  </si>
+  <si>
+    <t>301614477</t>
+  </si>
+  <si>
+    <t>23/07/2012</t>
+  </si>
+  <si>
+    <t>Tỉnh Long An</t>
+  </si>
+  <si>
+    <t>0914155295</t>
+  </si>
+  <si>
+    <t>huutin271@gmail.com</t>
+  </si>
+  <si>
+    <t>ấp 4, Phường 05, Quận 5, Thành Phố Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>ấp 4, Xã Lương Bình, Huyện Bến Lức, Tỉnh Long An</t>
+  </si>
+  <si>
+    <t>Tốt</t>
+  </si>
+  <si>
+    <t>Sinh viên</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giáo dục Thể chất
+</t>
+  </si>
+  <si>
+    <t>Trường Đại học Sư phạm Tp.HCM</t>
+  </si>
+  <si>
+    <t>1678491</t>
+  </si>
+  <si>
+    <t xml:space="preserve">có chứng nhận </t>
+  </si>
+  <si>
+    <t>có chứng nhận</t>
+  </si>
+  <si>
+    <t>Các trường hợp có ít nhất 05 năm công tác ở vị trí việc làm yêu cầu trình độ đào tạo đại học trở lên phù hợp với yêu cầu của vị trí việc làm cần tuyển dụng và có đóng bảo hiểm xã hội bắt buộc (không kể thời gian tập sự, thử việc, nếu có thời gian công tác có đóng bảo hiểm xã hội bắt buộc không liên tục mà chưa nhận trợ cấp bảo hiểm xã hội một lần thì được cộng dồn), gồm: Người ký hợp đồng lao động theo đúng quy định của pháp luật làm công việc chuyên môn, nghiệp vụ trong đơn vị sự nghiệp công lập tự bảo đảm chi thường xuyên, chi đầu tư và đơn vị sự nghiệp công lập tự bảo đảm chi thường xuyên hoặc đơn vị sự nghiệp ngoài công lập; Người hưởng lương trong lực lượng vũ trang (quân đội, công an) và người làm công tác cơ yếu; Cán bộ, công chức cấp xã; Người đang làm việc tại doanh nghiệp là công ty trách nhiệm hữu hạn một thành viên mà Nhà nước nắm giữ 100% vốn điều lệ hoặc doanh nghiệp mà Nhà nước nắm giữ trên 50% vốn điều lệ.</t>
+  </si>
+  <si>
+    <t>Huyện Bình Chánh</t>
+  </si>
+  <si>
+    <t>Quận 9</t>
+  </si>
+  <si>
+    <t>HT19_2</t>
+  </si>
+  <si>
+    <t>TD16</t>
+  </si>
+  <si>
+    <t>TRẦN DUY HƯNG</t>
+  </si>
+  <si>
+    <t>24/02/1996</t>
+  </si>
+  <si>
+    <t>025898999</t>
+  </si>
+  <si>
+    <t>24/05/2014</t>
+  </si>
+  <si>
+    <t>0987221721</t>
+  </si>
+  <si>
+    <t>hungtd242@gmail.com</t>
+  </si>
+  <si>
+    <t>Tỉnh Hà Nam</t>
+  </si>
+  <si>
+    <t>F2B, PHAN VĂN TRỊ, Phường 05, Quận Gò Vấp, Thành Phố Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>Nhân viên</t>
+  </si>
+  <si>
+    <t>Trường đại học Sư Phạm Tp.HCM</t>
+  </si>
+  <si>
+    <t>1675379</t>
+  </si>
+  <si>
+    <t>0387663</t>
+  </si>
+  <si>
+    <t>A2717887</t>
+  </si>
+  <si>
+    <t>Quận 12</t>
+  </si>
+  <si>
+    <t>Quận Phú Nhuận</t>
+  </si>
+  <si>
+    <t>HT19_3</t>
+  </si>
+  <si>
+    <t>TD17</t>
+  </si>
+  <si>
+    <t>Giáo dục quốc phòng</t>
+  </si>
+  <si>
+    <t>BÙI VĂN GIỎI</t>
+  </si>
+  <si>
+    <t>08/01/1987</t>
+  </si>
+  <si>
+    <t>241036249</t>
+  </si>
+  <si>
+    <t>12/04/2006</t>
+  </si>
+  <si>
+    <t>Tỉnh Đắk Lắk</t>
+  </si>
+  <si>
+    <t>0949954174</t>
+  </si>
+  <si>
+    <t>vangioisg86@gmail.com</t>
+  </si>
+  <si>
+    <t>Tỉnh Hà Tĩnh</t>
+  </si>
+  <si>
+    <t>Thôn 4, Phường 01, Quận Gò Vấp, Thành Phố Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>Thôn 4, Xã Ea Păl, Huyện Ea Kar, Tỉnh Đắk Lắk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giáo dục Quốc phòng An ninh
+</t>
+  </si>
+  <si>
+    <t>Đại học Sư Phạm Tp. Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>858944</t>
+  </si>
+  <si>
+    <t>Chứng chỉ: A, B, C được cấp trước ngày 15 tháng 12 năm 2016</t>
+  </si>
+  <si>
+    <t>A 1735036</t>
+  </si>
+  <si>
+    <t>A 1589085</t>
+  </si>
+  <si>
+    <t>Huyện Cần Giờ</t>
+  </si>
+  <si>
+    <t>HT19_4</t>
+  </si>
+  <si>
+    <t>TD18</t>
+  </si>
+  <si>
+    <t>Thiết bị, phòng thí nghiệm</t>
+  </si>
+  <si>
+    <t>LÊ TẤN THỊNH</t>
+  </si>
+  <si>
+    <t>20/04/1981</t>
+  </si>
+  <si>
+    <t>264142683</t>
+  </si>
+  <si>
+    <t>11/09/2011</t>
+  </si>
+  <si>
+    <t>Tỉnh Ninh Thuận</t>
+  </si>
+  <si>
+    <t>0907239729</t>
+  </si>
+  <si>
+    <t>letanthinh176@gmail.com</t>
+  </si>
+  <si>
+    <t>208 Trường Chinh, Phường 05, Quận 10, Thành Phố Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>208 Trường Chinh, Phường Văn Hải, Thành Phố Phan Rang-Tháp Chàm, Tỉnh Ninh Thuận</t>
+  </si>
+  <si>
+    <t>Tốt nghiệp Cao đẳng ngành khác</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thiết bị  Thí nghiệm
+</t>
+  </si>
+  <si>
+    <t>Liên thông chính qui</t>
+  </si>
+  <si>
+    <t>Trường đại học công nghiệp TP.HCM</t>
+  </si>
+  <si>
+    <t>Trung bình</t>
+  </si>
+  <si>
+    <t>A223297</t>
+  </si>
+  <si>
+    <t>12282</t>
+  </si>
+  <si>
+    <t>A187731</t>
+  </si>
+  <si>
+    <t>Quận 5</t>
+  </si>
+  <si>
+    <t>Quận 10</t>
+  </si>
+  <si>
+    <t>LT19_5</t>
+  </si>
+  <si>
+    <t>TD19</t>
+  </si>
+  <si>
+    <t>Thủ quỹ</t>
+  </si>
+  <si>
+    <t>LÊ THỊ CẨM TIÊN</t>
+  </si>
+  <si>
+    <t>13/07/1992</t>
+  </si>
+  <si>
+    <t>Nữ</t>
+  </si>
+  <si>
+    <t>331659003</t>
+  </si>
+  <si>
+    <t>02/03/2015</t>
+  </si>
+  <si>
+    <t>Tỉnh Vĩnh Long</t>
+  </si>
+  <si>
+    <t>0357151614</t>
+  </si>
+  <si>
+    <t>lethicamtien4492@gmail.com</t>
+  </si>
+  <si>
+    <t>Số nhà 110, ấp Long Công, Phường Phú Trung, Quận Tân Phú, Thành Phố Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>Số nhà 110, ấp Long Công, Xã Phú Lộc, Huyện Tam Bình, Tỉnh Vĩnh Long</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kế toán
+</t>
+  </si>
+  <si>
+    <t>Trường Cao Đẳng Kinh tế - Tài chính Vĩnh Long</t>
+  </si>
+  <si>
+    <t>B 157484</t>
+  </si>
+  <si>
+    <t>A 1163050</t>
+  </si>
+  <si>
+    <t>A 1272913</t>
+  </si>
+  <si>
+    <t>Quận Bình Tân</t>
+  </si>
+  <si>
+    <t>Quận Tân Phú</t>
+  </si>
+  <si>
+    <t>Huyện Hóc Môn</t>
+  </si>
+  <si>
+    <t>LT19_6</t>
+  </si>
+  <si>
+    <t>TD20</t>
+  </si>
+  <si>
+    <t>Ngữ văn</t>
+  </si>
+  <si>
+    <t>LÊ THỊ CÚC</t>
+  </si>
+  <si>
+    <t>23/08/1995</t>
+  </si>
+  <si>
+    <t>174809575</t>
+  </si>
+  <si>
+    <t>06/10/2012</t>
   </si>
   <si>
     <t>Tỉnh Thanh Hóa</t>
   </si>
   <si>
-    <t>28/17A, HT26, Phường Bến Nghé, Quận 1, Thành Phố Hồ Chí Minh</t>
-  </si>
-  <si>
-    <t>Tốt</t>
-  </si>
-  <si>
-    <t>Viên chức</t>
-  </si>
-  <si>
-    <t>Tốt nghiệp Đại học ngành khác</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phần mềm
+    <t>0962748267</t>
+  </si>
+  <si>
+    <t>lecuc230895@gmail.com</t>
+  </si>
+  <si>
+    <t>thôn 2, Phường Tân Sơn Nhì, Quận Tân Phú, Thành Phố Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>thôn 2, Xã Xuân Phong, Huyện Thọ Xuân, Tỉnh Thanh Hóa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sư phạm Ngữ văn
 </t>
   </si>
   <si>
-    <t>Chính quy</t>
-  </si>
-  <si>
-    <t>Đại học FPT</t>
-  </si>
-  <si>
-    <t>Tín chỉ</t>
-  </si>
-  <si>
-    <t>Trung bình khá</t>
-  </si>
-  <si>
-    <t>6.72</t>
-  </si>
-  <si>
-    <t>Tốt nghiệp chuyên ngành CNTT</t>
-  </si>
-  <si>
-    <t>FPT-0001</t>
-  </si>
-  <si>
-    <t>Không có</t>
-  </si>
-  <si>
-    <t>Bậc 4/ TRKI II/ DELF B2/ Đức B2 test DaF level 4/ HSK cấp 4/ JLPT N4/ Topik II-L4</t>
-  </si>
-  <si>
-    <t>31241</t>
-  </si>
-  <si>
-    <t>Người có tài năng, năng khiếu đặc biệt phù hợp với vị trí việc làm trong các ngành, lĩnh vực: Văn hóa, nghệ thuật, thể dục thể thao, các ngành nghề truyền thống.</t>
-  </si>
-  <si>
-    <t>Huyện Bình Chánh</t>
-  </si>
-  <si>
-    <t>Quận 8</t>
-  </si>
-  <si>
-    <t>Quận 4</t>
-  </si>
-  <si>
-    <t>02/07/2019</t>
+    <t>Trường Đại học Hồng Đức</t>
+  </si>
+  <si>
+    <t>HDT000566</t>
+  </si>
+  <si>
+    <t>1032046</t>
+  </si>
+  <si>
+    <t>A2515377</t>
+  </si>
+  <si>
+    <t>HT19_7</t>
   </si>
 </sst>
 </file>
@@ -325,7 +699,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:AS7"/>
+  <dimension ref="A2:AS13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -374,6 +748,8 @@
     <col min="41" max="41" width="16.8139234270368" customWidth="1"/>
     <col min="42" max="42" width="16.8139234270368" customWidth="1"/>
     <col min="43" max="43" width="16.8139234270368" customWidth="1"/>
+    <col min="44" max="44" width="12.2080830165318" customWidth="1"/>
+    <col min="45" max="45" width="15.1606499808175" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -543,10 +919,10 @@
       <c r="AQ6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AR6" s="0" t="s">
+      <c r="AR6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AS6" s="0" t="s">
+      <c r="AS6" s="4" t="s">
         <v>42</v>
       </c>
     </row>
@@ -588,10 +964,10 @@
         <v>54</v>
       </c>
       <c r="M7" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="N7" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="N7" s="0" t="s">
-        <v>56</v>
       </c>
       <c r="O7" s="0" t="s">
         <v>56</v>
@@ -600,10 +976,10 @@
         <v>57</v>
       </c>
       <c r="Q7" s="0">
-        <v>170</v>
+        <v>1.68</v>
       </c>
       <c r="R7" s="0">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="S7" s="0" t="s">
         <v>58</v>
@@ -621,67 +997,871 @@
         <v>62</v>
       </c>
       <c r="X7" s="0" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="Y7" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z7" s="0">
+        <v>2016</v>
+      </c>
+      <c r="AA7" s="0">
+        <v>7.34</v>
+      </c>
+      <c r="AC7" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD7" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE7" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF7" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG7" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH7" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI7" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ7" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK7" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL7" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM7" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN7" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO7" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="AP7" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="AQ7" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR7" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="AS7" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="N8" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="O8" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="P8" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q8" s="0">
+        <v>175</v>
+      </c>
+      <c r="R8" s="0">
+        <v>60</v>
+      </c>
+      <c r="S8" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="T8" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="U8" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="V8" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="W8" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="X8" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="Z7" s="0">
+      <c r="Y8" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z8" s="0">
+        <v>2019</v>
+      </c>
+      <c r="AA8" s="0">
+        <v>7.66</v>
+      </c>
+      <c r="AC8" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD8" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="AE8" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF8" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG8" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH8" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI8" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ8" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK8" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL8" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM8" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN8" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="AO8" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="AP8" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="AQ8" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="AR8" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="AS8" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N9" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="O9" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="P9" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q9" s="0">
+        <v>170</v>
+      </c>
+      <c r="R9" s="0">
+        <v>61</v>
+      </c>
+      <c r="S9" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="T9" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="U9" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="V9" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="W9" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="X9" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y9" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z9" s="0">
         <v>2018</v>
       </c>
-      <c r="AA7" s="0">
-        <v>6.72</v>
-      </c>
-      <c r="AC7" s="0" t="s">
+      <c r="AA9" s="0">
+        <v>7.46</v>
+      </c>
+      <c r="AC9" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD9" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AE9" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF9" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG9" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH9" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI9" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ9" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="AK9" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL9" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM9" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN9" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO9" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP9" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="AQ9" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR9" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="AS9" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="N10" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="O10" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="P10" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q10" s="0">
+        <v>175</v>
+      </c>
+      <c r="R10" s="0">
+        <v>68</v>
+      </c>
+      <c r="S10" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="T10" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="U10" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="V10" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="W10" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="X10" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y10" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="AD7" s="0" t="s">
+      <c r="Z10" s="0">
+        <v>2014</v>
+      </c>
+      <c r="AA10" s="0">
+        <v>2.58</v>
+      </c>
+      <c r="AC10" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="AE7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="AF7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="AG7" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH7" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="AI7" s="0" t="s">
+      <c r="AD10" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="AE10" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF10" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG10" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="AH10" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="AI10" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ10" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="AK10" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL10" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM10" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN10" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO10" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="AP10" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="AQ10" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="AR10" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="AS10" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="N11" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="O11" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="P11" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q11" s="0">
+        <v>169</v>
+      </c>
+      <c r="R11" s="0">
+        <v>82</v>
+      </c>
+      <c r="S11" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="T11" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="U11" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="V11" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="W11" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="X11" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y11" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z11" s="0">
+        <v>2010</v>
+      </c>
+      <c r="AA11" s="0">
+        <v>6.2</v>
+      </c>
+      <c r="AC11" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="AD11" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="AE11" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF11" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG11" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="AH11" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="AI11" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ11" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="AK11" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL11" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM11" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN11" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="AO11" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="AP11" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="AQ11" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="AR11" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="AS11" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="M12" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="N12" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="O12" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="P12" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q12" s="0">
+        <v>164</v>
+      </c>
+      <c r="R12" s="0">
+        <v>58</v>
+      </c>
+      <c r="S12" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="T12" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="U12" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="V12" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="W12" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="X12" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="Y12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z12" s="0">
+        <v>2015</v>
+      </c>
+      <c r="AA12" s="0">
+        <v>7.075</v>
+      </c>
+      <c r="AC12" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD12" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="AE12" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF12" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG12" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="AH12" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="AI12" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ12" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="AK12" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL12" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM12" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN12" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO12" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="AP12" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="AQ12" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="AR12" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="AS12" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="L13" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="M13" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="N13" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="O13" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="P13" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q13" s="0">
+        <v>160</v>
+      </c>
+      <c r="R13" s="0">
+        <v>47</v>
+      </c>
+      <c r="S13" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="T13" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="U13" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="V13" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="W13" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="X13" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="Y13" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z13" s="0">
+        <v>2017</v>
+      </c>
+      <c r="AA13" s="0">
+        <v>7.4</v>
+      </c>
+      <c r="AC13" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD13" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="AE13" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF13" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG13" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="AJ7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="AK7" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="AL7" s="0" t="s">
+      <c r="AH13" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="AI13" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="AM7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="AN7" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AO7" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="AP7" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="AQ7" s="0" t="s">
+      <c r="AJ13" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="AK13" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL13" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM13" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN13" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO13" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="AR7" s="0">
-        <v>4</v>
-      </c>
-      <c r="AS7" s="0" t="s">
-        <v>75</v>
+      <c r="AP13" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="AQ13" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="AR13" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="AS13" s="0" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>